<commit_message>
mofication du convertiseur avec ouverture du doss
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
   <si>
     <t>TEST</t>
   </si>
@@ -157,6 +157,30 @@
   </si>
   <si>
     <t>4.85</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Identification:</t>
+  </si>
+  <si>
+    <t>07.03.22</t>
+  </si>
+  <si>
+    <t>68.0 kg</t>
+  </si>
+  <si>
+    <t>3.55</t>
+  </si>
+  <si>
+    <t>-0.41</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>1.45</t>
   </si>
 </sst>
 </file>
@@ -514,7 +538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -605,6 +629,50 @@
         <v>23</v>
       </c>
       <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3">
         <v>0</v>
       </c>
     </row>

</xml_diff>